<commit_message>
fix issue with garage/producer location
</commit_message>
<xml_diff>
--- a/py/assets/config.xlsx
+++ b/py/assets/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\ICBC_E-Stamp_Tool\py\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB29FF1-B351-4139-A386-BA5A8CAFECFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA3FB2F-8B8E-4E40-9204-9A4AC699772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1980" windowWidth="16815" windowHeight="10335" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICBC E-Stamp and Copy Tool" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Producer Code</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>Input_Path</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Two scripts included:</t>
-  </si>
-  <si>
-    <t>README: https://github.com/WebDevBernard/ICBC_E-Stamp_Tool</t>
   </si>
   <si>
     <r>
@@ -147,12 +141,15 @@
       <t xml:space="preserve"> – Limited to stamping and copying 10 pdfs at a time.  It will check duplicates before stamping or copying.  It works as long as your policy documents are downloaded to the Download folder.</t>
     </r>
   </si>
+  <si>
+    <t>Readme: https://github.com/WebDevBernard/ICBC_E-Stamp_Tool</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,21 +160,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -209,16 +191,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -226,15 +222,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -244,12 +257,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,70 +586,70 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:2" ht="18.75">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -646,78 +663,78 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="18.75">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -731,50 +748,50 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="101.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="101.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="8" customFormat="1" ht="18.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" s="4" customFormat="1" ht="18.75">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="45">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:1" ht="60">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="45">
+      <c r="A10" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="30">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="45">
-      <c r="A5" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30">
-      <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:1" ht="60">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="45">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>